<commit_message>
Updated admin and user
</commit_message>
<xml_diff>
--- a/webui/resources/TestData/TestData.xlsx
+++ b/webui/resources/TestData/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Autothon 2019\webui\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1BFE9C0-6310-4EE9-9CB6-A848662CA2AE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F9F74B-25DA-4E00-B49C-2A335119DF7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{8E1EB67A-26BC-4AC1-AD9F-3E751CE15994}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{8E1EB67A-26BC-4AC1-AD9F-3E751CE15994}"/>
   </bookViews>
   <sheets>
     <sheet name="Logins" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>UserType</t>
   </si>
@@ -101,6 +101,12 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>https://authothon-nagarro-frontend-b07.azurewebsites.net</t>
   </si>
 </sst>
 </file>
@@ -145,13 +151,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -469,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C51287FE-583F-455D-A62A-5E3E830DEE26}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -500,7 +507,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
         <v>8</v>
@@ -532,8 +539,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F1509C-F66F-49E2-B932-98A71B5CA3CA}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -589,8 +596,8 @@
       <c r="F2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G2">
-        <v>3</v>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>